<commit_message>
Multiple changes since late March. Added inventory and 1min-binned files to git tracking. - Sept: Added choice of basemaps. Changed github repo url to https://github.com/amazon-riverbgc. Tested successfully with new conda env, holovizgen with the latest package versions, and with JupyterLab 2 (2.15). - April: Added customized web app HTML title. Changed default app tab to be the map browser tab. - Created pinned version of environment.yml, and eliminated version pinning from the latter
</commit_message>
<xml_diff>
--- a/data/inventories/licor_sensor_df_describe_stats.xlsx
+++ b/data/inventories/licor_sensor_df_describe_stats.xlsx
@@ -390,13 +390,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3842952</v>
+        <v>4615394</v>
       </c>
       <c r="C2" t="n">
-        <v>3842952</v>
+        <v>4615394</v>
       </c>
       <c r="D2" t="n">
-        <v>3842952</v>
+        <v>4615394</v>
       </c>
     </row>
     <row r="3">
@@ -406,13 +406,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2809.982714608458</v>
+        <v>2631.216873112026</v>
       </c>
       <c r="C3" t="n">
-        <v>50.88743118831574</v>
+        <v>50.98690042280242</v>
       </c>
       <c r="D3" t="n">
-        <v>100.528447508582</v>
+        <v>100.5246395323996</v>
       </c>
     </row>
     <row r="4">
@@ -422,13 +422,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1769.488471214198</v>
+        <v>1687.396185362857</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4415339261773154</v>
+        <v>0.4607548801340078</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8902983830926915</v>
+        <v>0.8281038551113546</v>
       </c>
     </row>
     <row r="5">
@@ -438,13 +438,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124.7</v>
+        <v>-50</v>
       </c>
       <c r="C5" t="n">
         <v>39.23</v>
       </c>
       <c r="D5" t="n">
-        <v>81.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6">
@@ -454,7 +454,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1534.17</v>
+        <v>1520.96</v>
       </c>
       <c r="C6" t="n">
         <v>50.55</v>
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2286.74</v>
+        <v>2083.16</v>
       </c>
       <c r="C7" t="n">
-        <v>50.55</v>
+        <v>50.58</v>
       </c>
       <c r="D7" t="n">
         <v>100.51</v>
@@ -486,13 +486,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3900.1</v>
+        <v>3639.5375</v>
       </c>
       <c r="C8" t="n">
         <v>51.44</v>
       </c>
       <c r="D8" t="n">
-        <v>100.71</v>
+        <v>100.72</v>
       </c>
     </row>
     <row r="9">
@@ -502,13 +502,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>12998.16</v>
+        <v>119615.22</v>
       </c>
       <c r="C9" t="n">
-        <v>51.73</v>
+        <v>51.85</v>
       </c>
       <c r="D9" t="n">
-        <v>106.74</v>
+        <v>120.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>